<commit_message>
Updates so output if finalized
Mostly work on updates to summarize output to send out, but some other code was updated
</commit_message>
<xml_diff>
--- a/Data/Attribute_LifeStage_Crosswalk.xlsx
+++ b/Data/Attribute_LifeStage_Crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34142215-02C4-4DF1-A994-FE0536A5C39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B96F425-AB97-4E5F-B395-EA244A439E67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="132" windowWidth="19092" windowHeight="12228" xr2:uid="{611DF7DE-642B-4840-9A75-6536BEE518E4}"/>
+    <workbookView xWindow="2628" yWindow="744" windowWidth="20172" windowHeight="11544" xr2:uid="{611DF7DE-642B-4840-9A75-6536BEE518E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="45">
   <si>
     <t>Species</t>
   </si>
@@ -60,9 +82,6 @@
     <t>% Fines/Embeddedness</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>BT Natal Rearing</t>
   </si>
   <si>
@@ -126,9 +145,6 @@
     <t>Pools- Deep Pools</t>
   </si>
   <si>
-    <t>Predators- Adult</t>
-  </si>
-  <si>
     <t>Predators- Juveniles</t>
   </si>
   <si>
@@ -172,6 +188,12 @@
   </si>
   <si>
     <t>Predators Fry</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Predators- Adults</t>
   </si>
 </sst>
 </file>
@@ -618,18 +640,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA5C33B-3429-4218-AF97-9225DAF5FE2F}">
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:F176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="36.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="36.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,434 +668,523 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="str" cm="1">
+        <f t="array" ref="F2:F27">_xlfn.UNIQUE(C2:C136)</f>
+        <v>Flow- Summer Base Flow</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Contaminants</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Food- Food Web Resources</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" t="str">
+        <v>Harassment</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Pool Quantity &amp; Quality</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" t="str">
+        <v>Temperature- Rearing</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="F8" t="str">
+        <v>Brook Trout</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Coarse Substrate</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Cover- Undercut Banks</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Cover- Wood</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="str">
+        <v xml:space="preserve">Off-Channel- Floodplain </v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="F13" t="str">
+        <v>Off-Channel- Side-Channels</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Predators- Juveniles</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Cover- Boulders</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="F16" t="str">
+        <v>Pools- Deep Pools</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Predators- Adults</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Temperature- Adult Holding</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="D19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="str">
+        <v>% Fines/Embeddedness</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="D20" s="4"/>
+      <c r="F20" t="str">
+        <v>Flow- Scour</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="4"/>
+      <c r="F21" t="str">
+        <v>Icing</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Entrainment- Fry</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Hybridization</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="F24" t="str">
+        <v>Superimposition</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Temperature- Adult Spawning</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="F26" t="str">
+        <v>Entrainment- Summer Rearing</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Predators Fry</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1078,13 +1192,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1092,25 +1206,27 @@
         <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1118,13 +1234,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1132,13 +1248,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1146,10 +1262,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D40" s="4"/>
     </row>
@@ -1158,10 +1274,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D41" s="4"/>
     </row>
@@ -1169,11 +1285,11 @@
       <c r="A42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>8</v>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D42" s="4"/>
     </row>
@@ -1182,691 +1298,721 @@
         <v>4</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C47" s="3" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C48" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C49" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D68" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D71" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D74" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D75" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D76" s="4"/>
+      <c r="D76" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D78" s="4"/>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D79" s="4"/>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D80" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D81" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D86" s="4"/>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>15</v>
@@ -1875,307 +2021,339 @@
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D102" s="4"/>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D103" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D104" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D105" s="4"/>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D107" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D109" s="4"/>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D110" s="4"/>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D112" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D113" s="4"/>
+      <c r="D113" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D114" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D115" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D116" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D117" s="4"/>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D118" s="4"/>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D119" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D120" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D121" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D122" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D123" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D124" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D125" s="4"/>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>34</v>
@@ -2187,130 +2365,140 @@
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D127" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>36</v>
+      <c r="A128" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D128" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D129" s="4"/>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="6" t="s">
-        <v>43</v>
+      <c r="A130" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D130" s="4"/>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D131" s="4"/>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D132" s="4"/>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D133" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D134" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D135" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D136" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="4"/>
-      <c r="C137" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="C137" s="3"/>
       <c r="D137" s="4"/>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Developed code and generated new output for WebMap
new output has each individual row having unique reach-habitat attribute-life stage (second ouput also has unique output for species)
</commit_message>
<xml_diff>
--- a/Data/Attribute_LifeStage_Crosswalk.xlsx
+++ b/Data/Attribute_LifeStage_Crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90C2CC7-37EA-4EC1-A58B-10CC03B51770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C5069F-713C-4DE3-8AAF-7D207075550C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1224" yWindow="552" windowWidth="20172" windowHeight="11544" xr2:uid="{611DF7DE-642B-4840-9A75-6536BEE518E4}"/>
+    <workbookView xWindow="588" yWindow="384" windowWidth="16848" windowHeight="10824" xr2:uid="{611DF7DE-642B-4840-9A75-6536BEE518E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="42">
   <si>
     <t>Species</t>
   </si>
@@ -141,15 +141,6 @@
     <t>Summer Rearing</t>
   </si>
   <si>
-    <t>Entrainment- Fry</t>
-  </si>
-  <si>
-    <t>Entrainment- Summer Rearing</t>
-  </si>
-  <si>
-    <t>Hybridization</t>
-  </si>
-  <si>
     <t>Smolt Outmigration</t>
   </si>
   <si>
@@ -169,6 +160,9 @@
   </si>
   <si>
     <t>Predators- Adults</t>
+  </si>
+  <si>
+    <t>Entrainment/Stranding</t>
   </si>
 </sst>
 </file>
@@ -618,11 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA5C33B-3429-4218-AF97-9225DAF5FE2F}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -658,10 +651,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -672,10 +665,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -686,10 +679,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -701,7 +694,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -712,10 +705,10 @@
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -727,7 +720,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -739,7 +732,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -750,10 +743,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -764,34 +757,38 @@
         <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -803,7 +800,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -814,10 +811,10 @@
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -828,10 +825,10 @@
         <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -843,7 +840,7 @@
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -854,10 +851,10 @@
         <v>10</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -868,36 +865,36 @@
         <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -909,7 +906,7 @@
       </c>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
@@ -920,10 +917,10 @@
         <v>20</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -934,10 +931,10 @@
         <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
@@ -949,7 +946,7 @@
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
@@ -960,10 +957,10 @@
         <v>25</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -975,7 +972,7 @@
       </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -986,12 +983,12 @@
         <v>29</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
@@ -1003,29 +1000,31 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
@@ -1036,10 +1035,10 @@
         <v>19</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1050,10 +1049,10 @@
         <v>21</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1064,10 +1063,10 @@
         <v>25</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
@@ -1078,10 +1077,10 @@
         <v>26</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -1089,13 +1088,13 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -1106,10 +1105,10 @@
         <v>28</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
@@ -1120,10 +1119,10 @@
         <v>6</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -1134,10 +1133,10 @@
         <v>8</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
@@ -1148,10 +1147,10 @@
         <v>10</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
@@ -1163,7 +1162,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1174,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>4</v>
       </c>
@@ -1187,7 +1186,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
@@ -1199,7 +1198,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>30</v>
       </c>
@@ -1211,7 +1210,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>30</v>
       </c>
@@ -1225,19 +1224,17 @@
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>30</v>
       </c>
@@ -1245,11 +1242,11 @@
         <v>32</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>30</v>
       </c>
@@ -1261,7 +1258,7 @@
       </c>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>30</v>
       </c>
@@ -1275,21 +1272,19 @@
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>13</v>
@@ -1307,11 +1302,11 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>30</v>
       </c>
@@ -1323,7 +1318,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>30</v>
       </c>
@@ -1335,7 +1330,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>30</v>
       </c>
@@ -1347,7 +1342,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>30</v>
       </c>
@@ -1359,7 +1354,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>30</v>
       </c>
@@ -1367,11 +1362,11 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>30</v>
       </c>
@@ -1383,19 +1378,19 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>30</v>
       </c>
@@ -1407,7 +1402,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>30</v>
       </c>
@@ -1419,7 +1414,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1426,7 @@
       </c>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>30</v>
       </c>
@@ -1443,7 +1438,7 @@
       </c>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>30</v>
       </c>
@@ -1455,7 +1450,7 @@
       </c>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>30</v>
       </c>
@@ -1467,7 +1462,7 @@
       </c>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>30</v>
       </c>
@@ -1475,11 +1470,11 @@
         <v>5</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>30</v>
       </c>
@@ -1491,7 +1486,7 @@
       </c>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>30</v>
       </c>
@@ -1502,10 +1497,10 @@
         <v>24</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>30</v>
       </c>
@@ -1513,13 +1508,13 @@
         <v>5</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>30</v>
       </c>
@@ -1527,13 +1522,13 @@
         <v>5</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>30</v>
       </c>
@@ -1544,10 +1539,10 @@
         <v>10</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>30</v>
       </c>
@@ -1558,7 +1553,7 @@
         <v>12</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1569,39 +1564,41 @@
         <v>33</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D74" s="4"/>
+      <c r="D74" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>30</v>
       </c>
@@ -1609,13 +1606,13 @@
         <v>33</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>30</v>
       </c>
@@ -1627,7 +1624,7 @@
       </c>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>30</v>
       </c>
@@ -1639,7 +1636,7 @@
       </c>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>30</v>
       </c>
@@ -1651,7 +1648,7 @@
       </c>
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>30</v>
       </c>
@@ -1662,10 +1659,10 @@
         <v>24</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>30</v>
       </c>
@@ -1676,10 +1673,10 @@
         <v>25</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>30</v>
       </c>
@@ -1690,10 +1687,10 @@
         <v>27</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>30</v>
       </c>
@@ -1705,7 +1702,7 @@
       </c>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>30</v>
       </c>
@@ -1717,7 +1714,7 @@
       </c>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>30</v>
       </c>
@@ -1731,31 +1728,29 @@
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D86" s="4"/>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>30</v>
       </c>
@@ -1767,7 +1762,7 @@
       </c>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>30</v>
       </c>
@@ -1779,7 +1774,7 @@
       </c>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>30</v>
       </c>
@@ -1791,7 +1786,7 @@
       </c>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>30</v>
       </c>
@@ -1803,9 +1798,9 @@
       </c>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>18</v>
@@ -1815,9 +1810,9 @@
       </c>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>32</v>
@@ -1829,35 +1824,35 @@
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>32</v>
@@ -1866,12 +1861,12 @@
         <v>23</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>32</v>
@@ -1881,59 +1876,57 @@
       </c>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D101" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D101" s="4"/>
+    </row>
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>13</v>
@@ -1943,9 +1936,9 @@
       </c>
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>13</v>
@@ -1954,12 +1947,12 @@
         <v>21</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>13</v>
@@ -1968,12 +1961,12 @@
         <v>25</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>13</v>
@@ -1983,21 +1976,21 @@
       </c>
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>13</v>
@@ -2006,26 +1999,26 @@
         <v>28</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>5</v>
@@ -2035,9 +2028,9 @@
       </c>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>5</v>
@@ -2047,9 +2040,9 @@
       </c>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>5</v>
@@ -2058,12 +2051,12 @@
         <v>12</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>5</v>
@@ -2072,12 +2065,12 @@
         <v>17</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>5</v>
@@ -2086,12 +2079,12 @@
         <v>19</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>5</v>
@@ -2100,12 +2093,12 @@
         <v>21</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>5</v>
@@ -2114,12 +2107,12 @@
         <v>22</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>33</v>
@@ -2128,12 +2121,12 @@
         <v>10</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>33</v>
@@ -2145,59 +2138,61 @@
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D118" s="4"/>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D120" s="4"/>
-    </row>
-    <row r="121" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D120" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>33</v>
@@ -2206,12 +2201,12 @@
         <v>19</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>33</v>
@@ -2220,12 +2215,12 @@
         <v>20</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>33</v>
@@ -2234,12 +2229,12 @@
         <v>23</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>33</v>
@@ -2249,9 +2244,9 @@
       </c>
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>33</v>
@@ -2261,9 +2256,9 @@
       </c>
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>33</v>
@@ -2272,12 +2267,12 @@
         <v>27</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>33</v>
@@ -2286,12 +2281,12 @@
         <v>29</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>31</v>
@@ -2301,9 +2296,9 @@
       </c>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>31</v>
@@ -2315,21 +2310,19 @@
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D131" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D131" s="4"/>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>31</v>
@@ -2339,9 +2332,9 @@
       </c>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>31</v>
@@ -2350,12 +2343,12 @@
         <v>17</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>31</v>
@@ -2364,12 +2357,12 @@
         <v>22</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>31</v>
@@ -2378,12 +2371,12 @@
         <v>24</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>31</v>
@@ -2392,10 +2385,10 @@
         <v>23</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="4"/>
       <c r="C137" s="3"/>
@@ -2441,18 +2434,7 @@
     <row r="175" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="176" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:D137" xr:uid="{DAB5F8B1-7139-46E7-9A73-93F8C37D8656}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Cover- Boulders"/>
-        <filter val="Cover- Undercut Banks"/>
-        <filter val="Cover- Wood"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:D132">
-      <sortCondition ref="C1:C137"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D137" xr:uid="{DAB5F8B1-7139-46E7-9A73-93F8C37D8656}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated scripts for output to send to Aspect for WebMap
Included output for A) send Aspect for data queries in WebMap and B) for outward facing table for each reach
</commit_message>
<xml_diff>
--- a/Data/Attribute_LifeStage_Crosswalk.xlsx
+++ b/Data/Attribute_LifeStage_Crosswalk.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C5069F-713C-4DE3-8AAF-7D207075550C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17743FCE-84DF-4D82-80C9-C7750C5F48A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="384" windowWidth="16848" windowHeight="10824" xr2:uid="{611DF7DE-642B-4840-9A75-6536BEE518E4}"/>
+    <workbookView xWindow="1248" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{611DF7DE-642B-4840-9A75-6536BEE518E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$136</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="42">
   <si>
     <t>Species</t>
   </si>
@@ -279,7 +279,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +296,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA5C33B-3429-4218-AF97-9225DAF5FE2F}">
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="97" workbookViewId="0">
+      <selection activeCell="B126" sqref="A126:XFD126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,10 +646,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>39</v>
@@ -656,79 +657,75 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -736,8 +733,8 @@
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
@@ -764,11 +761,11 @@
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>7</v>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
@@ -778,11 +775,11 @@
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>39</v>
@@ -790,39 +787,37 @@
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>39</v>
@@ -830,53 +825,49 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>39</v>
@@ -884,13 +875,13 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -899,12 +890,14 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -914,7 +907,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>39</v>
@@ -925,36 +918,34 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>39</v>
@@ -962,29 +953,29 @@
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
@@ -1000,25 +991,25 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>39</v>
@@ -1026,69 +1017,61 @@
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>13</v>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>39</v>
@@ -1099,10 +1082,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>39</v>
@@ -1113,38 +1096,34 @@
         <v>4</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>39</v>
@@ -1152,63 +1131,69 @@
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>5</v>
+      <c r="B42" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
@@ -1218,7 +1203,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D45" s="4"/>
     </row>
@@ -1227,7 +1212,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>16</v>
@@ -1239,67 +1224,73 @@
         <v>30</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>16</v>
@@ -1311,10 +1302,10 @@
         <v>30</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D53" s="4"/>
     </row>
@@ -1323,46 +1314,52 @@
         <v>30</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D56" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D57" s="4"/>
     </row>
@@ -1371,10 +1368,10 @@
         <v>30</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D58" s="4"/>
     </row>
@@ -1383,67 +1380,75 @@
         <v>30</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>19</v>
@@ -1452,25 +1457,27 @@
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D66" s="4"/>
     </row>
@@ -1479,10 +1486,10 @@
         <v>30</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D67" s="4"/>
     </row>
@@ -1494,63 +1501,55 @@
         <v>5</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>39</v>
@@ -1558,13 +1557,13 @@
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>39</v>
@@ -1572,27 +1571,25 @@
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>39</v>
@@ -1606,123 +1603,125 @@
         <v>33</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D77" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D78" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D80" s="4"/>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D83" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D85" s="4"/>
     </row>
@@ -1731,10 +1730,10 @@
         <v>30</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D86" s="4"/>
     </row>
@@ -1746,25 +1745,27 @@
         <v>31</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D88" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>31</v>
@@ -1772,69 +1773,71 @@
       <c r="C89" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D89" s="4"/>
+      <c r="D89" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D91" s="4"/>
+      <c r="D91" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
@@ -1844,7 +1847,7 @@
         <v>32</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>39</v>
@@ -1855,7 +1858,7 @@
         <v>37</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>23</v>
@@ -1869,110 +1872,114 @@
         <v>37</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D97" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>32</v>
+        <v>4</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D98" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D101" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D103" s="4"/>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D104" s="4"/>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D105" s="4"/>
     </row>
@@ -1981,36 +1988,36 @@
         <v>37</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D106" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D107" s="4"/>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>39</v>
@@ -2018,37 +2025,39 @@
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D110" s="4"/>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>39</v>
@@ -2059,10 +2068,10 @@
         <v>37</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>39</v>
@@ -2073,24 +2082,22 @@
         <v>37</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D113" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D113" s="4"/>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>39</v>
@@ -2098,53 +2105,51 @@
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D115" s="4"/>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D116" s="4"/>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D117" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D118" s="4"/>
     </row>
@@ -2153,66 +2158,58 @@
         <v>37</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D119" s="4"/>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D120" s="4"/>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D121" s="4"/>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D122" s="4"/>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>39</v>
@@ -2223,10 +2220,10 @@
         <v>37</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>39</v>
@@ -2240,107 +2237,115 @@
         <v>33</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D125" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D126" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>33</v>
+      <c r="A127" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>33</v>
+      <c r="A128" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D128" s="4"/>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B129" s="6" t="s">
-        <v>31</v>
+      <c r="B129" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D129" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D130" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D131" s="4"/>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B132" s="6" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D132" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>39</v>
@@ -2348,52 +2353,37 @@
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D134" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D134" s="4"/>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="5"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="3"/>
-      <c r="D137" s="4"/>
-    </row>
+      <c r="A136" s="5"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2432,9 +2422,12 @@
     <row r="173" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="174" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="175" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:D137" xr:uid="{DAB5F8B1-7139-46E7-9A73-93F8C37D8656}"/>
+  <autoFilter ref="A1:D136" xr:uid="{DAB5F8B1-7139-46E7-9A73-93F8C37D8656}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D136">
+      <sortCondition ref="C1:C136"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>